<commit_message>
Template changes cckh prod,sand
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="181">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -884,10 +884,11 @@
     <t xml:space="preserve">Club</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml</t>
+    <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,
+Coke ESP 330ml </t>
   </si>
   <si>
-    <t xml:space="preserve">8847100562715,8847100562746,8847100567574,8847100566898,8847100565389,8847100562234,8847100562234,8847100565389,8847100567468,8847100565389</t>
+    <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5</t>
   </si>
   <si>
     <t xml:space="preserve">Sprite 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET</t>
@@ -911,10 +912,10 @@
     <t xml:space="preserve">8847100567352,8847100564184,8847100564061,8847100905883,8847100568793</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanta Grape  330ml,Fanta Redberry 330ml,Fanta Blueberry 330ml,Fanta Blueberry 390ml</t>
+    <t xml:space="preserve">Fanta Grape  330ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100560117,8847100561329,8847100568588,8847100568175,8847100563880,8847100567215,8847100561725</t>
+    <t xml:space="preserve">8847100560117</t>
   </si>
   <si>
     <t xml:space="preserve">Samurai Strawberry 330ml,Samurai Fruity 330ml,Samurai Strawberry 480ml,Samurai Fruity 480ml</t>
@@ -923,10 +924,10 @@
     <t xml:space="preserve">8847100566591,8847100566607,8847100566874,8847100566676,8847100566867,8847100567864</t>
   </si>
   <si>
-    <t xml:space="preserve">Dasani 350ml,Dasani 500ml,Dasani 1.5L PET</t>
+    <t xml:space="preserve">Dasani 350ml,Dasani 500ml,Dasani 1.5L PETDasani 550ml,Dasani Mineral 500ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100560025,8847100568526,8847100562111,8847100567784</t>
+    <t xml:space="preserve">8847100560025,8847100568526,8847100562111,8851959905999,8847100567784</t>
   </si>
   <si>
     <t xml:space="preserve">Aquarius 330ml Can,Aquarius 330ml Sleek Can,Aquarius 390ml PET</t>
@@ -974,13 +975,10 @@
     <t xml:space="preserve">Sprite Zero 330ml Can</t>
   </si>
   <si>
-    <t xml:space="preserve">Mutant Green 330ml Can,
-Mutant Black 330ml Can,
-Mutant Green 400ml PET,
-Mutant Yellow 400ml PET</t>
+    <t xml:space="preserve">Mutant Green 330ml Can,Mutant Black 330ml Can,Mutant Green 400ml PET,Mutant Yellow 400ml PET,Mutant Red 330ml Can</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100566650,8847100568601,8847100568595,8847100568618</t>
+    <t xml:space="preserve">8847100566650,8847100568601,8847100568595,8847100568618,8847100565943</t>
   </si>
   <si>
     <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
@@ -998,7 +996,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1074,8 +1072,14 @@
       <charset val="177"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1375,7 +1379,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1512,10 +1516,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1536,12 +1536,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="3" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1692,7 +1700,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1800,7 +1808,7 @@
   </sheetPr>
   <dimension ref="1:39"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
@@ -1808,27 +1816,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.73279352226721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.0121457489879"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.7287449392713"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="78.5951417004049"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="44.8056680161943"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6113360323887"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="35.748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.1619433198381"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.1619433198381"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.5263157894737"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="62.1943319838057"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="79.2672064777328"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.0971659919028"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="62.7732793522267"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.2105263157895"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="3" width="12.9757085020243"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34547,32 +34555,32 @@
   </sheetPr>
   <dimension ref="1:21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.81376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="39.7854251012146"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="30.6072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="3.79352226720648"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="11.8744939271255"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="11.5060728744939"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="21" width="4.40485829959514"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="3.79352226720648"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="21" width="6.48987854251012"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="40.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="3.74898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="21" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="3.74898785425101"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="21" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="21" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="21" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="21" width="8.32793522267206"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="21" width="5.51417004048583"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="21" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="21" width="14.9311740890688"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="21" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="21" width="6.53441295546559"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="21" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="21" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="21" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="21" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="21" width="9.63967611336032"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="21" width="4.2834008097166"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="21" width="4.89878542510122"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="21" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="21" width="4.92712550607287"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="21" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -36668,7 +36676,7 @@
       <c r="K5" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="L5" s="33" t="s">
         <v>139</v>
       </c>
       <c r="M5" s="33" t="s">
@@ -36692,838 +36700,838 @@
       <c r="S5" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="68.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="36" t="s">
+    <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="39" t="n">
+      <c r="E6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="39" t="n">
+      <c r="F6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="39" t="n">
+      <c r="G6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="H6" s="39" t="n">
+      <c r="H6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="39" t="n">
+      <c r="I6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="J6" s="39" t="n">
+      <c r="J6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="39" t="n">
+      <c r="K6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="L6" s="39" t="n">
+      <c r="L6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="M6" s="39" t="n">
+      <c r="M6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="N6" s="39" t="n">
+      <c r="N6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="O6" s="39" t="n">
+      <c r="O6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="P6" s="39" t="n">
+      <c r="P6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" s="39" t="n">
+      <c r="Q6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="R6" s="39" t="n">
+      <c r="R6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="S6" s="39" t="n">
+      <c r="S6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="T6" s="39" t="n">
+      <c r="T6" s="38" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="39" t="n">
+      <c r="E7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="39" t="n">
+      <c r="F7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="39" t="n">
+      <c r="G7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="39" t="n">
+      <c r="H7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I7" s="39" t="n">
+      <c r="I7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="39" t="n">
+      <c r="J7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K7" s="39" t="n">
+      <c r="K7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L7" s="39" t="n">
+      <c r="L7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M7" s="39" t="n">
+      <c r="M7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="39" t="n">
+      <c r="N7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O7" s="39" t="n">
+      <c r="O7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P7" s="39" t="n">
+      <c r="P7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q7" s="39" t="n">
+      <c r="Q7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R7" s="39" t="n">
+      <c r="R7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S7" s="39" t="n">
+      <c r="S7" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T7" s="39" t="n">
+      <c r="T7" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="39" t="n">
+      <c r="E8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="39" t="n">
+      <c r="F8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="39" t="n">
+      <c r="G8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="39" t="n">
+      <c r="H8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I8" s="39" t="n">
+      <c r="I8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J8" s="39" t="n">
+      <c r="J8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K8" s="39" t="n">
+      <c r="K8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L8" s="39" t="n">
+      <c r="L8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M8" s="39" t="n">
+      <c r="M8" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P8" s="39" t="s">
+      <c r="P8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q8" s="39" t="s">
+      <c r="Q8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R8" s="39" t="s">
+      <c r="R8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S8" s="39" t="s">
+      <c r="S8" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T8" s="39" t="s">
+      <c r="T8" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="39" t="n">
+      <c r="E9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="39" t="n">
+      <c r="F9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="39" t="n">
+      <c r="G9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="39" t="n">
+      <c r="H9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I9" s="39" t="n">
+      <c r="I9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="39" t="n">
+      <c r="J9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="39" t="n">
+      <c r="K9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L9" s="39" t="n">
+      <c r="L9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M9" s="39" t="n">
+      <c r="M9" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q9" s="39" t="s">
+      <c r="Q9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R9" s="39" t="s">
+      <c r="R9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S9" s="39" t="s">
+      <c r="S9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T9" s="39" t="s">
+      <c r="T9" s="38" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="50.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="36" t="s">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="39" t="n">
+      <c r="E10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="39" t="n">
+      <c r="F10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="39" t="n">
+      <c r="G10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H10" s="39" t="n">
+      <c r="H10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I10" s="39" t="n">
+      <c r="I10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J10" s="39" t="n">
+      <c r="J10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K10" s="39" t="n">
+      <c r="K10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L10" s="39" t="n">
+      <c r="L10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M10" s="39" t="n">
+      <c r="M10" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="P10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="R10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="S10" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="T10" s="39" t="s">
-        <v>154</v>
+      <c r="N10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="P10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="R10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="S10" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="T10" s="38" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="E11" s="39" t="n">
+      <c r="E11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="39" t="n">
+      <c r="F11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="39" t="n">
+      <c r="G11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="39" t="n">
+      <c r="H11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I11" s="39" t="n">
+      <c r="I11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J11" s="39" t="n">
+      <c r="J11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K11" s="39" t="n">
+      <c r="K11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L11" s="39" t="n">
+      <c r="L11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M11" s="39" t="n">
+      <c r="M11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N11" s="39" t="n">
+      <c r="N11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O11" s="39" t="n">
+      <c r="O11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P11" s="39" t="n">
+      <c r="P11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q11" s="39" t="n">
+      <c r="Q11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R11" s="39" t="n">
+      <c r="R11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S11" s="39" t="n">
+      <c r="S11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T11" s="39" t="n">
+      <c r="T11" s="38" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="36" t="s">
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="39" t="n">
+      <c r="E12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="39" t="n">
+      <c r="F12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="39" t="n">
+      <c r="G12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="39" t="n">
+      <c r="H12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I12" s="39" t="n">
+      <c r="I12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J12" s="39" t="n">
+      <c r="J12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K12" s="39" t="n">
+      <c r="K12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L12" s="39" t="n">
+      <c r="L12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M12" s="39" t="n">
+      <c r="M12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N12" s="39" t="n">
+      <c r="N12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O12" s="39" t="n">
+      <c r="O12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P12" s="39" t="n">
+      <c r="P12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q12" s="39" t="n">
+      <c r="Q12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R12" s="39" t="n">
+      <c r="R12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S12" s="39" t="n">
+      <c r="S12" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T12" s="39" t="n">
+      <c r="T12" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="39" t="n">
+      <c r="E13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="39" t="n">
+      <c r="F13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="39" t="n">
+      <c r="G13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="H13" s="39" t="n">
+      <c r="H13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="39" t="n">
+      <c r="I13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="J13" s="39" t="n">
+      <c r="J13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="K13" s="39" t="n">
+      <c r="K13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="L13" s="39" t="n">
+      <c r="L13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="M13" s="39" t="n">
+      <c r="M13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="N13" s="39" t="n">
+      <c r="N13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="O13" s="39" t="n">
+      <c r="O13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="P13" s="39" t="n">
+      <c r="P13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="Q13" s="39" t="n">
+      <c r="Q13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="R13" s="39" t="n">
+      <c r="R13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="S13" s="39" t="n">
+      <c r="S13" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="T13" s="39" t="n">
+      <c r="T13" s="38" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="39" t="n">
+      <c r="E14" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="39" t="n">
+      <c r="F14" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="39" t="n">
+      <c r="G14" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N14" s="39" t="s">
+      <c r="N14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O14" s="39" t="s">
+      <c r="O14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P14" s="39" t="s">
+      <c r="P14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q14" s="39" t="s">
+      <c r="Q14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R14" s="39" t="s">
+      <c r="R14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S14" s="39" t="s">
+      <c r="S14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T14" s="39" t="s">
+      <c r="T14" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="E15" s="39" t="n">
+      <c r="E15" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="39" t="n">
+      <c r="F15" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="39" t="n">
+      <c r="G15" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="39" t="s">
+      <c r="H15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I15" s="39" t="s">
+      <c r="I15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N15" s="39" t="s">
+      <c r="N15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O15" s="39" t="s">
+      <c r="O15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P15" s="39" t="s">
+      <c r="P15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q15" s="39" t="s">
+      <c r="Q15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R15" s="39" t="s">
+      <c r="R15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S15" s="39" t="s">
+      <c r="S15" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T15" s="39" t="s">
+      <c r="T15" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="36" t="s">
         <v>169</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E16" s="39" t="n">
+      <c r="E16" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="39" t="n">
+      <c r="F16" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="39" t="n">
+      <c r="G16" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="I16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="K16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L16" s="39" t="s">
+      <c r="L16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M16" s="39" t="s">
+      <c r="M16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N16" s="39" t="s">
+      <c r="N16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P16" s="39" t="s">
+      <c r="P16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q16" s="39" t="s">
+      <c r="Q16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R16" s="39" t="s">
+      <c r="R16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S16" s="39" t="s">
+      <c r="S16" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T16" s="39" t="s">
+      <c r="T16" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="36" t="s">
         <v>171</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="39" t="n">
+      <c r="E17" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F17" s="39" t="n">
+      <c r="F17" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="39" t="n">
+      <c r="G17" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M17" s="39" t="s">
+      <c r="M17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N17" s="39" t="s">
+      <c r="N17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O17" s="39" t="s">
+      <c r="O17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P17" s="39" t="s">
+      <c r="P17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q17" s="39" t="s">
+      <c r="Q17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R17" s="39" t="s">
+      <c r="R17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S17" s="39" t="s">
+      <c r="S17" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T17" s="39" t="s">
+      <c r="T17" s="38" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="36" t="s">
+    <row r="18" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="36" t="s">
         <v>173</v>
       </c>
       <c r="D18" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="F18" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="G18" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" s="39" t="s">
+      <c r="E18" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="I18" s="39" t="s">
+      <c r="F18" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="G18" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="K18" s="39" t="s">
+      <c r="H18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="I18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M18" s="39" t="s">
+      <c r="J18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N18" s="39" t="s">
+      <c r="K18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="O18" s="39" t="s">
+      <c r="L18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="P18" s="39" t="s">
+      <c r="M18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="Q18" s="39" t="s">
+      <c r="N18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R18" s="39" t="s">
+      <c r="O18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="S18" s="39" t="s">
+      <c r="P18" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="T18" s="39" t="s">
+      <c r="Q18" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="R18" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="S18" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="T18" s="38" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="36" t="s">
         <v>175</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="39" t="s">
+      <c r="L19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="M19" s="39" t="s">
+      <c r="M19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N19" s="39" t="n">
+      <c r="N19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O19" s="39" t="n">
+      <c r="O19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P19" s="39" t="n">
+      <c r="P19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q19" s="39" t="n">
+      <c r="Q19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R19" s="39" t="n">
+      <c r="R19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S19" s="39" t="n">
+      <c r="S19" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T19" s="39" t="n">
+      <c r="T19" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>122</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -37532,111 +37540,111 @@
       <c r="D20" s="10" t="n">
         <v>8847100562364</v>
       </c>
-      <c r="E20" s="39" t="n">
+      <c r="E20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F20" s="39" t="n">
+      <c r="F20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="39" t="n">
+      <c r="G20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H20" s="39" t="n">
+      <c r="H20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I20" s="39" t="n">
+      <c r="I20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J20" s="39" t="n">
+      <c r="J20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K20" s="39" t="n">
+      <c r="K20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L20" s="39" t="n">
+      <c r="L20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M20" s="39" t="n">
+      <c r="M20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N20" s="39" t="n">
+      <c r="N20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O20" s="39" t="n">
+      <c r="O20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P20" s="39" t="n">
+      <c r="P20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q20" s="39" t="n">
+      <c r="Q20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R20" s="39" t="n">
+      <c r="R20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S20" s="39" t="n">
+      <c r="S20" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T20" s="39" t="n">
+      <c r="T20" s="38" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="36" t="s">
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="39" t="n">
+      <c r="E21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="39" t="n">
+      <c r="F21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="39" t="n">
+      <c r="G21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="H21" s="39" t="n">
+      <c r="H21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="I21" s="39" t="n">
+      <c r="I21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J21" s="39" t="n">
+      <c r="J21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="K21" s="39" t="n">
+      <c r="K21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="L21" s="39" t="n">
+      <c r="L21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="M21" s="39" t="n">
+      <c r="M21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="N21" s="39" t="n">
+      <c r="N21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="O21" s="39" t="n">
+      <c r="O21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="P21" s="39" t="n">
+      <c r="P21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="Q21" s="39" t="n">
+      <c r="Q21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="R21" s="39" t="n">
+      <c r="R21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="S21" s="39" t="n">
+      <c r="S21" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="T21" s="39" t="n">
+      <c r="T21" s="38" t="n">
         <v>3</v>
       </c>
     </row>
@@ -37670,22 +37678,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.26315789473684"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6315789473684"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="5.26315789473684"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.48987854251012"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.48987854251012"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.44939271255061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.51417004048583"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="4.89878542510122"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.24696356275304"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="5.24696356275304"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="4.92712550607287"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37727,7 +37735,7 @@
       <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="42"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="25" t="s">
         <v>180</v>
       </c>
@@ -37748,7 +37756,7 @@
       <c r="R3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="42"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="26" t="s">
         <v>128</v>
       </c>
@@ -37771,7 +37779,7 @@
       <c r="R4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="32" t="s">
@@ -37780,7 +37788,7 @@
       <c r="D5" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="45" t="s">
         <v>134</v>
       </c>
       <c r="F5" s="32" t="s">
@@ -37795,7 +37803,7 @@
       <c r="I5" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="33" t="s">
         <v>139</v>
       </c>
       <c r="K5" s="33" t="s">
@@ -37819,166 +37827,166 @@
       <c r="Q5" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="46" t="n">
+      <c r="C6" s="47" t="n">
         <v>1.25</v>
       </c>
-      <c r="D6" s="47" t="n">
+      <c r="D6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="48" t="n">
+      <c r="E6" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="46" t="n">
+      <c r="F6" s="47" t="n">
         <v>0.75</v>
       </c>
-      <c r="G6" s="49" t="n">
+      <c r="G6" s="50" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="49" t="n">
+      <c r="H6" s="50" t="n">
         <v>0.75</v>
       </c>
-      <c r="I6" s="49" t="n">
+      <c r="I6" s="50" t="n">
         <v>0.75</v>
       </c>
-      <c r="J6" s="49" t="n">
+      <c r="J6" s="50" t="n">
         <v>0.75</v>
       </c>
-      <c r="K6" s="49" t="n">
+      <c r="K6" s="50" t="n">
         <v>0.75</v>
       </c>
-      <c r="L6" s="47" t="n">
+      <c r="L6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="47" t="n">
+      <c r="M6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="47" t="n">
+      <c r="N6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="47" t="n">
+      <c r="O6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="P6" s="47" t="n">
+      <c r="P6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="47" t="n">
+      <c r="Q6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="R6" s="50" t="n">
+      <c r="R6" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="52" t="n">
+      <c r="C7" s="53" t="n">
         <v>1.25</v>
       </c>
-      <c r="D7" s="53" t="n">
+      <c r="D7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="55" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="52" t="n">
+      <c r="F7" s="53" t="n">
         <v>0.75</v>
       </c>
-      <c r="G7" s="55" t="n">
+      <c r="G7" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="H7" s="55" t="n">
+      <c r="H7" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="I7" s="55" t="n">
+      <c r="I7" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="J7" s="55" t="n">
+      <c r="J7" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="K7" s="55" t="n">
+      <c r="K7" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="L7" s="53" t="n">
+      <c r="L7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="53" t="n">
+      <c r="M7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="53" t="n">
+      <c r="N7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="53" t="n">
+      <c r="O7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="53" t="n">
+      <c r="P7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="53" t="n">
+      <c r="Q7" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="R7" s="56" t="n">
+      <c r="R7" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="58" t="n">
+      <c r="C8" s="59" t="n">
         <v>2.5</v>
       </c>
-      <c r="D8" s="59" t="n">
+      <c r="D8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="60" t="n">
+      <c r="E8" s="61" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="58" t="n">
+      <c r="F8" s="59" t="n">
         <v>1.5</v>
       </c>
-      <c r="G8" s="61" t="n">
+      <c r="G8" s="62" t="n">
         <v>1.5</v>
       </c>
-      <c r="H8" s="61" t="n">
+      <c r="H8" s="62" t="n">
         <v>1.5</v>
       </c>
-      <c r="I8" s="61" t="n">
+      <c r="I8" s="62" t="n">
         <v>1.5</v>
       </c>
-      <c r="J8" s="61" t="n">
+      <c r="J8" s="62" t="n">
         <v>1.5</v>
       </c>
-      <c r="K8" s="61" t="n">
+      <c r="K8" s="62" t="n">
         <v>1.5</v>
       </c>
-      <c r="L8" s="59" t="n">
+      <c r="L8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="59" t="n">
+      <c r="M8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="N8" s="59" t="n">
+      <c r="N8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="59" t="n">
+      <c r="O8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="59" t="n">
+      <c r="P8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="59" t="n">
+      <c r="Q8" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="R8" s="62" t="n">
+      <c r="R8" s="63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38012,24 +38020,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6113360323887"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.40485829959514"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.753036437247"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6315789473684"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.89878542510122"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="4.40485829959514"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.48987854251012"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.48987854251012"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.44939271255061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.51417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="1" width="4.40485829959514"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.92712550607287"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="1" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38073,8 +38081,8 @@
       <c r="S2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="25" t="s">
         <v>180</v>
       </c>
@@ -38095,8 +38103,8 @@
       <c r="S3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="42"/>
-      <c r="C4" s="63"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="26" t="s">
         <v>128</v>
       </c>
@@ -38119,13 +38127,13 @@
       <c r="S4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="67" t="s">
         <v>132</v>
       </c>
       <c r="E5" s="33" t="s">
@@ -38170,399 +38178,399 @@
       <c r="R5" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="69" t="n">
+      <c r="D6" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="69" t="n">
+      <c r="E6" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="70" t="n">
+      <c r="F6" s="71" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="71" t="n">
+      <c r="G6" s="72" t="n">
         <v>0.5</v>
       </c>
-      <c r="H6" s="69" t="n">
+      <c r="H6" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="69" t="n">
+      <c r="I6" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="J6" s="69" t="n">
+      <c r="J6" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="K6" s="69" t="n">
+      <c r="K6" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="L6" s="69" t="n">
+      <c r="L6" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="M6" s="72" t="n">
+      <c r="M6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="N6" s="72" t="n">
+      <c r="N6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="O6" s="72" t="n">
+      <c r="O6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="P6" s="72" t="n">
+      <c r="P6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="72" t="n">
+      <c r="Q6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="R6" s="72" t="n">
+      <c r="R6" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="S6" s="73" t="n">
+      <c r="S6" s="74" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="69" t="n">
+      <c r="D7" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="69" t="n">
+      <c r="E7" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="70" t="n">
+      <c r="F7" s="71" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="71" t="n">
+      <c r="G7" s="72" t="n">
         <v>0.5</v>
       </c>
-      <c r="H7" s="69" t="n">
+      <c r="H7" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="I7" s="69" t="n">
+      <c r="I7" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="J7" s="69" t="n">
+      <c r="J7" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="K7" s="69" t="n">
+      <c r="K7" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="L7" s="69" t="n">
+      <c r="L7" s="70" t="n">
         <v>0.5</v>
       </c>
-      <c r="M7" s="72" t="n">
+      <c r="M7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="N7" s="72" t="n">
+      <c r="N7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="O7" s="72" t="n">
+      <c r="O7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="P7" s="72" t="n">
+      <c r="P7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="72" t="n">
+      <c r="Q7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="R7" s="72" t="n">
+      <c r="R7" s="73" t="n">
         <v>0.5</v>
       </c>
-      <c r="S7" s="73" t="n">
+      <c r="S7" s="74" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="69" t="n">
+      <c r="D8" s="70" t="n">
         <v>2.5</v>
       </c>
-      <c r="E8" s="69" t="n">
+      <c r="E8" s="70" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="70" t="n">
+      <c r="F8" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="71" t="n">
+      <c r="G8" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="69" t="n">
+      <c r="H8" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="69" t="n">
+      <c r="I8" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="69" t="n">
+      <c r="J8" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="69" t="n">
+      <c r="K8" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="69" t="n">
+      <c r="L8" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="M8" s="72" t="n">
+      <c r="M8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="N8" s="72" t="n">
+      <c r="N8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="O8" s="72" t="n">
+      <c r="O8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="P8" s="72" t="n">
+      <c r="P8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="72" t="n">
+      <c r="Q8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="R8" s="72" t="n">
+      <c r="R8" s="73" t="n">
         <v>1.5</v>
       </c>
-      <c r="S8" s="73" t="n">
+      <c r="S8" s="74" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="68" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="69" t="n">
+      <c r="D9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="69" t="n">
+      <c r="E9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="70" t="n">
+      <c r="F9" s="71" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="71" t="n">
+      <c r="G9" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="69" t="n">
+      <c r="H9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="69" t="n">
+      <c r="I9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="69" t="n">
+      <c r="J9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="69" t="n">
+      <c r="K9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="69" t="n">
+      <c r="L9" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="72" t="n">
+      <c r="M9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="72" t="n">
+      <c r="N9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="72" t="n">
+      <c r="O9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="72" t="n">
+      <c r="P9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="72" t="n">
+      <c r="Q9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="R9" s="72" t="n">
+      <c r="R9" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="73" t="n">
+      <c r="S9" s="74" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="69" t="n">
+      <c r="D10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="69" t="n">
+      <c r="E10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="70" t="n">
+      <c r="F10" s="71" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="71" t="n">
+      <c r="G10" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="69" t="n">
+      <c r="H10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="69" t="n">
+      <c r="I10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="69" t="n">
+      <c r="J10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="69" t="n">
+      <c r="K10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="69" t="n">
+      <c r="L10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="72" t="n">
+      <c r="M10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="72" t="n">
+      <c r="N10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="72" t="n">
+      <c r="O10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="72" t="n">
+      <c r="P10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="72" t="n">
+      <c r="Q10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="R10" s="72" t="n">
+      <c r="R10" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="S10" s="73" t="n">
+      <c r="S10" s="74" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="69" t="n">
+      <c r="D11" s="70" t="n">
         <v>2.5</v>
       </c>
-      <c r="E11" s="69" t="n">
+      <c r="E11" s="70" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="70" t="n">
+      <c r="F11" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="76" t="n">
+      <c r="G11" s="77" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="77" t="n">
+      <c r="H11" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="77" t="n">
+      <c r="I11" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="J11" s="77" t="n">
+      <c r="J11" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="77" t="n">
+      <c r="K11" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="L11" s="77" t="n">
+      <c r="L11" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="M11" s="77" t="n">
+      <c r="M11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="77" t="n">
+      <c r="N11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="77" t="n">
+      <c r="O11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="P11" s="77" t="n">
+      <c r="P11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="77" t="n">
+      <c r="Q11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="R11" s="77" t="n">
+      <c r="R11" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="S11" s="78" t="n">
+      <c r="S11" s="79" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="80" t="n">
+      <c r="D12" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="80" t="n">
+      <c r="E12" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="81" t="n">
+      <c r="F12" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="82" t="n">
+      <c r="G12" s="83" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="83" t="n">
+      <c r="H12" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="83" t="n">
+      <c r="I12" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="83" t="n">
+      <c r="J12" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="83" t="n">
+      <c r="K12" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="83" t="n">
+      <c r="L12" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="84" t="s">
+      <c r="M12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="N12" s="84" t="s">
+      <c r="N12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="O12" s="84" t="s">
+      <c r="O12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="P12" s="84" t="s">
+      <c r="P12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="Q12" s="84" t="s">
+      <c r="Q12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="R12" s="84" t="s">
+      <c r="R12" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="85" t="s">
+      <c r="S12" s="86" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes in Availability template
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="183">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -884,23 +884,95 @@
     <t xml:space="preserve">Club</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,
-Coke ESP 330ml </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,
+Coke ESP 330ml,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Coca Cola Coffee 330ml</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8847100562395</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Sprite 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sprite 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sprite Zero 330ml Can</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">8851959905944,8847100562104,8847100561459,8847100563736,8847100568793</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8847100561459,8851959905944,8847100563736,8847100562104,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8847100562364</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Fanta Orange 330ml,Fanta Orange 390ml,Fanta Orange 500ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100560094,8847100561244,8847100564603,8847100905883,8847100567376</t>
+    <t xml:space="preserve">8847100560094,8847100561244,8847100564603</t>
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
@@ -909,19 +981,87 @@
     <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 390ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100567352,8847100564184,8847100564061,8847100905883,8847100568793</t>
+    <t xml:space="preserve">8847100564184,8847100564061</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanta Grape  330ml</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fanta Redberry 330ml,Fanta Blueberry 330ml,Fanta Blueberry 390ml,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fanta Grape  330ml,Fanta Redberry 330ml,Fanta Blueberry 330ml,Fanta +C 390ml,Fanta +C 330ml</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">8847100560117</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8847100561329,8847100563880_d,8847100568175,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8847100560117,8847100561329,8847100568588,8847100567215,8847100561725</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Samurai Strawberry 330ml,Samurai Fruity 330ml,Samurai Strawberry 480ml,Samurai Fruity 480ml</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Samurai Strawberry 330ml,Samurai Fruity 330ml,Samurai Strawberry 480ml,Samurai Fruity 480ml,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Mutant Green 330ml Can, Mutant Black 330ml Can,Mutant Green 400ml PET,Mutant Yellow 400ml PET,Mutant Red 330ml Can,Mutant Red 400ml PET</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">8847100566591,8847100566607,8847100566874,8847100566676,8847100566867,8847100567864</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8847100566591,8847100566607,8847100566874,8847100566676,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8847100566650,8847100568601,8847100568595,8847100568618,8847100565943,8847100565952</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Dasani 350ml,Dasani 500ml,Dasani 1.5L PETDasani 550ml,Dasani Mineral 500ml</t>
@@ -966,19 +1106,13 @@
     <t xml:space="preserve">8847100563149,8847100568830</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanta Orange 330ml,Fanta Fruit Punch 330ml,Fanta Grape  330ml,Fanta Redberry 330ml,Fanta Blueberry 330ml,Fanta Blueberry 390ml,Fanta Orange 390ml,Fanta Fruit Punch 390ml,Fanta Orange 500ml</t>
+    <t xml:space="preserve">Minute Maid (Can or PET) Single Serve</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100560094,8847100567352,8847100560117,8847100561329,8847100568588,8847100568175,8847100561244,8847100564184,8847100564603</t>
+    <t xml:space="preserve">Minute Maid Grape 330ml Can,Minute Maid Apple 330ml Can,Minute Maid Orange Mango 330ml Can</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprite Zero 330ml Can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutant Green 330ml Can,Mutant Black 330ml Can,Mutant Green 400ml PET,Mutant Yellow 400ml PET,Mutant Red 330ml Can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100566650,8847100568601,8847100568595,8847100568618,8847100565943</t>
+    <t xml:space="preserve">8847100569837,8847100562951,8847100562388,</t>
   </si>
   <si>
     <t xml:space="preserve">Schweppe (Can) Single Serve</t>
@@ -1008,7 +1142,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1082,6 +1216,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1385,7 +1530,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1542,8 +1687,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1554,11 +1703,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1718,7 +1875,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1834,26 +1991,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.2024291497976"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="79.9109311740891"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.4210526315789"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="80.5546558704453"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.7408906882591"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="63.3076923076923"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="63.8421052631579"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -34571,20 +34728,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:22"/>
+  <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="40.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="47.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="40.7044534412955"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.3846153846154"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="21" width="3.74898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="21" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="21" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="21" width="3.74898785425101"/>
@@ -34594,8 +34751,8 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="21" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="21" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="21" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="21" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="21" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="21" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="21" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="21" width="4.2834008097166"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="21" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="21" width="8.78542510121457"/>
@@ -36722,7 +36879,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="79.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
         <v>22</v>
       </c>
@@ -36781,7 +36938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="41.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
         <v>29</v>
       </c>
@@ -36840,7 +36997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="35" t="s">
         <v>31</v>
       </c>
@@ -36899,7 +37056,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="35" t="s">
         <v>33</v>
       </c>
@@ -36958,14 +37115,14 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="35" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="40" t="s">
         <v>158</v>
       </c>
       <c r="E10" s="38" t="n">
@@ -37017,7 +37174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="35" t="s">
         <v>37</v>
       </c>
@@ -37319,7 +37476,7 @@
       <c r="C16" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="41" t="s">
         <v>170</v>
       </c>
       <c r="E16" s="38" t="n">
@@ -37378,7 +37535,7 @@
       <c r="C17" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="42" t="s">
         <v>172</v>
       </c>
       <c r="E17" s="38" t="n">
@@ -37437,7 +37594,7 @@
       <c r="C18" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="42" t="s">
         <v>174</v>
       </c>
       <c r="E18" s="38" t="s">
@@ -37489,15 +37646,15 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="36" t="s">
+    <row r="19" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="C19" s="39" t="s">
         <v>176</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>177</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>154</v>
@@ -37526,205 +37683,89 @@
       <c r="M19" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="N19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="O19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="P19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="R19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="S19" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="T19" s="38" t="n">
-        <v>3</v>
+      <c r="N19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="O19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="R19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="S19" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="T19" s="38" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D20" s="10" t="n">
-        <v>8847100562364</v>
-      </c>
-      <c r="E20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="G20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="H20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="I20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="J20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="K20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="L20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="M20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="N20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="O20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="P20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="R20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="S20" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="T20" s="38" t="n">
-        <v>3</v>
+    <row r="20" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="J20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="L20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="N20" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="O20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="P20" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="R20" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="S20" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="T20" s="48" t="n">
+        <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="F21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="G21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="H21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="I21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="J21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="K21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="L21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="M21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="N21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="O21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="P21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="R21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="S21" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="T21" s="38" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="I22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="J22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="K22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="M22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="N22" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="O22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="P22" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="R22" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="S22" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="T22" s="45" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B3:D4"/>
@@ -37756,7 +37797,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.2793522267206"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.24696356275304"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
@@ -37766,8 +37807,8 @@
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.57085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="1" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.31983805668016"/>
@@ -37812,9 +37853,9 @@
       <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="46"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -37833,7 +37874,7 @@
       <c r="R3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="46"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="26" t="s">
         <v>128</v>
       </c>
@@ -37856,7 +37897,7 @@
       <c r="R4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="50" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="32" t="s">
@@ -37865,7 +37906,7 @@
       <c r="D5" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="51" t="s">
         <v>134</v>
       </c>
       <c r="F5" s="32" t="s">
@@ -37909,161 +37950,161 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="50" t="n">
+      <c r="C6" s="53" t="n">
         <v>1.25</v>
       </c>
-      <c r="D6" s="51" t="n">
+      <c r="D6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="52" t="n">
+      <c r="E6" s="55" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="50" t="n">
+      <c r="F6" s="53" t="n">
         <v>0.75</v>
       </c>
-      <c r="G6" s="53" t="n">
+      <c r="G6" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="53" t="n">
+      <c r="H6" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="I6" s="53" t="n">
+      <c r="I6" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="J6" s="53" t="n">
+      <c r="J6" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="K6" s="53" t="n">
+      <c r="K6" s="56" t="n">
         <v>0.75</v>
       </c>
-      <c r="L6" s="51" t="n">
+      <c r="L6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="51" t="n">
+      <c r="M6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="51" t="n">
+      <c r="N6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="51" t="n">
+      <c r="O6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="P6" s="51" t="n">
+      <c r="P6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="51" t="n">
+      <c r="Q6" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="R6" s="54" t="n">
+      <c r="R6" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="56" t="n">
+      <c r="C7" s="59" t="n">
         <v>1.25</v>
       </c>
-      <c r="D7" s="57" t="n">
+      <c r="D7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="58" t="n">
+      <c r="E7" s="61" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="56" t="n">
+      <c r="F7" s="59" t="n">
         <v>0.75</v>
       </c>
-      <c r="G7" s="59" t="n">
+      <c r="G7" s="62" t="n">
         <v>0.75</v>
       </c>
-      <c r="H7" s="59" t="n">
+      <c r="H7" s="62" t="n">
         <v>0.75</v>
       </c>
-      <c r="I7" s="59" t="n">
+      <c r="I7" s="62" t="n">
         <v>0.75</v>
       </c>
-      <c r="J7" s="59" t="n">
+      <c r="J7" s="62" t="n">
         <v>0.75</v>
       </c>
-      <c r="K7" s="59" t="n">
+      <c r="K7" s="62" t="n">
         <v>0.75</v>
       </c>
-      <c r="L7" s="57" t="n">
+      <c r="L7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="57" t="n">
+      <c r="M7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="57" t="n">
+      <c r="N7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="57" t="n">
+      <c r="O7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="57" t="n">
+      <c r="P7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="57" t="n">
+      <c r="Q7" s="60" t="n">
         <v>0</v>
       </c>
-      <c r="R7" s="60" t="n">
+      <c r="R7" s="63" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="62" t="n">
+      <c r="C8" s="65" t="n">
         <v>2.5</v>
       </c>
-      <c r="D8" s="63" t="n">
+      <c r="D8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="64" t="n">
+      <c r="E8" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="62" t="n">
+      <c r="F8" s="65" t="n">
         <v>1.5</v>
       </c>
-      <c r="G8" s="65" t="n">
+      <c r="G8" s="68" t="n">
         <v>1.5</v>
       </c>
-      <c r="H8" s="65" t="n">
+      <c r="H8" s="68" t="n">
         <v>1.5</v>
       </c>
-      <c r="I8" s="65" t="n">
+      <c r="I8" s="68" t="n">
         <v>1.5</v>
       </c>
-      <c r="J8" s="65" t="n">
+      <c r="J8" s="68" t="n">
         <v>1.5</v>
       </c>
-      <c r="K8" s="65" t="n">
+      <c r="K8" s="68" t="n">
         <v>1.5</v>
       </c>
-      <c r="L8" s="63" t="n">
+      <c r="L8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="63" t="n">
+      <c r="M8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="N8" s="63" t="n">
+      <c r="N8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="63" t="n">
+      <c r="O8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="63" t="n">
+      <c r="P8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="63" t="n">
+      <c r="Q8" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="R8" s="66" t="n">
+      <c r="R8" s="69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38098,8 +38139,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6761133603239"/>
@@ -38110,8 +38151,8 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="9.31983805668016"/>
@@ -38158,10 +38199,10 @@
       <c r="S2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -38180,8 +38221,8 @@
       <c r="S3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="46"/>
-      <c r="C4" s="67"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="26" t="s">
         <v>128</v>
       </c>
@@ -38204,13 +38245,13 @@
       <c r="S4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="73" t="s">
         <v>132</v>
       </c>
       <c r="E5" s="33" t="s">
@@ -38260,394 +38301,394 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="73" t="n">
+      <c r="D6" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="73" t="n">
+      <c r="E6" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="74" t="n">
+      <c r="F6" s="77" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="75" t="n">
+      <c r="G6" s="78" t="n">
         <v>0.5</v>
       </c>
-      <c r="H6" s="73" t="n">
+      <c r="H6" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="73" t="n">
+      <c r="I6" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="J6" s="73" t="n">
+      <c r="J6" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="K6" s="73" t="n">
+      <c r="K6" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="L6" s="73" t="n">
+      <c r="L6" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="M6" s="76" t="n">
+      <c r="M6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="N6" s="76" t="n">
+      <c r="N6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="O6" s="76" t="n">
+      <c r="O6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="P6" s="76" t="n">
+      <c r="P6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="76" t="n">
+      <c r="Q6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="R6" s="76" t="n">
+      <c r="R6" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="S6" s="77" t="n">
+      <c r="S6" s="80" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="73" t="n">
+      <c r="D7" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="73" t="n">
+      <c r="E7" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="74" t="n">
+      <c r="F7" s="77" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="75" t="n">
+      <c r="G7" s="78" t="n">
         <v>0.5</v>
       </c>
-      <c r="H7" s="73" t="n">
+      <c r="H7" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="I7" s="73" t="n">
+      <c r="I7" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="J7" s="73" t="n">
+      <c r="J7" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="K7" s="73" t="n">
+      <c r="K7" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="L7" s="73" t="n">
+      <c r="L7" s="76" t="n">
         <v>0.5</v>
       </c>
-      <c r="M7" s="76" t="n">
+      <c r="M7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="N7" s="76" t="n">
+      <c r="N7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="O7" s="76" t="n">
+      <c r="O7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="P7" s="76" t="n">
+      <c r="P7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="76" t="n">
+      <c r="Q7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="R7" s="76" t="n">
+      <c r="R7" s="79" t="n">
         <v>0.5</v>
       </c>
-      <c r="S7" s="77" t="n">
+      <c r="S7" s="80" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="73" t="n">
+      <c r="D8" s="76" t="n">
         <v>2.5</v>
       </c>
-      <c r="E8" s="73" t="n">
+      <c r="E8" s="76" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="74" t="n">
+      <c r="F8" s="77" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="75" t="n">
+      <c r="G8" s="78" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="73" t="n">
+      <c r="H8" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="73" t="n">
+      <c r="I8" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="73" t="n">
+      <c r="J8" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="73" t="n">
+      <c r="K8" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="73" t="n">
+      <c r="L8" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="M8" s="76" t="n">
+      <c r="M8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="N8" s="76" t="n">
+      <c r="N8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="O8" s="76" t="n">
+      <c r="O8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="P8" s="76" t="n">
+      <c r="P8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="76" t="n">
+      <c r="Q8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="R8" s="76" t="n">
+      <c r="R8" s="79" t="n">
         <v>1.5</v>
       </c>
-      <c r="S8" s="77" t="n">
+      <c r="S8" s="80" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="74" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="73" t="n">
+      <c r="D9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="73" t="n">
+      <c r="E9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="74" t="n">
+      <c r="F9" s="77" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="75" t="n">
+      <c r="G9" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="73" t="n">
+      <c r="H9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="73" t="n">
+      <c r="I9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="73" t="n">
+      <c r="J9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="73" t="n">
+      <c r="K9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="73" t="n">
+      <c r="L9" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="76" t="n">
+      <c r="M9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="76" t="n">
+      <c r="N9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="76" t="n">
+      <c r="O9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="76" t="n">
+      <c r="P9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="76" t="n">
+      <c r="Q9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="R9" s="76" t="n">
+      <c r="R9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="77" t="n">
+      <c r="S9" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="73" t="n">
+      <c r="D10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="73" t="n">
+      <c r="E10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="74" t="n">
+      <c r="F10" s="77" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="75" t="n">
+      <c r="G10" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="73" t="n">
+      <c r="H10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="73" t="n">
+      <c r="I10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="73" t="n">
+      <c r="J10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="73" t="n">
+      <c r="K10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="73" t="n">
+      <c r="L10" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="76" t="n">
+      <c r="M10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="76" t="n">
+      <c r="N10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="76" t="n">
+      <c r="O10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="76" t="n">
+      <c r="P10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="76" t="n">
+      <c r="Q10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="R10" s="76" t="n">
+      <c r="R10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="S10" s="77" t="n">
+      <c r="S10" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="73" t="n">
+      <c r="D11" s="76" t="n">
         <v>2.5</v>
       </c>
-      <c r="E11" s="73" t="n">
+      <c r="E11" s="76" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="74" t="n">
+      <c r="F11" s="77" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="80" t="n">
+      <c r="G11" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="81" t="n">
+      <c r="H11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="81" t="n">
+      <c r="I11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="J11" s="81" t="n">
+      <c r="J11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="81" t="n">
+      <c r="K11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="L11" s="81" t="n">
+      <c r="L11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="M11" s="81" t="n">
+      <c r="M11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="81" t="n">
+      <c r="N11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="81" t="n">
+      <c r="O11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="P11" s="81" t="n">
+      <c r="P11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="81" t="n">
+      <c r="Q11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="R11" s="81" t="n">
+      <c r="R11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="S11" s="82" t="n">
+      <c r="S11" s="85" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="84" t="n">
+      <c r="D12" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="84" t="n">
+      <c r="E12" s="87" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="85" t="n">
+      <c r="F12" s="88" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="86" t="n">
+      <c r="G12" s="89" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="87" t="n">
+      <c r="H12" s="90" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="87" t="n">
+      <c r="I12" s="90" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="87" t="n">
+      <c r="J12" s="90" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="87" t="n">
+      <c r="K12" s="90" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="87" t="n">
+      <c r="L12" s="90" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="88" t="s">
+      <c r="M12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="N12" s="88" t="s">
+      <c r="N12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="O12" s="88" t="s">
+      <c r="O12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="P12" s="88" t="s">
+      <c r="P12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="Q12" s="88" t="s">
+      <c r="Q12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="R12" s="88" t="s">
+      <c r="R12" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="89" t="s">
+      <c r="S12" s="92" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-6224 - CCKH - Template update - KPI Names into English from Local language was updated by mistake. Updating back to English for visibility and cooler
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="183">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -891,17 +891,44 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coca Cola Coffee 330ml,Coke 240ml,Coca-cola 250ml Can,Coke Vanilla 330ml,</t>
+      <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coca Cola Coffee 330ml,Coke 240ml,Coca-cola 250ml Can,Coke Vanilla 330ml
+</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,88471005623958851959905876,8847100562999,8847100565495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite 330ml Can,Sprite Zero 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET,Sprite 330ml Sleek Can,Sprite 240ml Slim Can,Sprite 250ml Can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561459,8847100562364,8847100563736,8851959905944,8847100562104,8847100568793,8851959905906,8847100568847</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Coca Cola 350ml
+      <t xml:space="preserve">Fanta Orange 330ml,Fanta Orange 390ml,Fanta Orange 500ml,Fanta Orange 240ml Slim Can,Fanta Orange 250ml Can
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100560094,8847100561244,8847100564603,
+8851959905883,8847100564799</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 390ml,Fanta Fruit Punch 330ml Sleek Can,Fanta Fruit Punch 240ml Slim Can,Fanta Fruit Punch 250ml Can
 </t>
     </r>
   </si>
@@ -913,147 +940,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,88471005623958851959905876,8847100562999,8847100565495,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100561015</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sprite 330ml Can,Sprite Zero 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET,Sprite 330ml Sleek Can,Sprite 240ml Slim Can,Sprite 250ml Can,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sprite 350ml
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100561459,8847100562364,8847100563736,8851959905944,8847100562104,8847100568793,8851959905906,8847100568847,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100561022</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Orange 330ml,Fanta Orange 390ml,Fanta Orange 500ml,Fanta Orange 240ml Slim Can,Fanta Orange 250ml Can,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Orange 350ml
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100560094,8847100561244,8847100564603,
-8851959905883,8847100564799,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100561046_0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 390ml,Fanta Fruit Punch 330ml Sleek Can,Fanta Fruit Punch 240ml Slim Can,Fanta Fruit Punch 250ml Can,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Fruit Punch 350ml
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100564061,8847100564184,8847100564061,8851959133187,8847100569011,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100561046_0
+      <t xml:space="preserve">8847100564061,8847100564184,8847100564061,8851959133187,8847100569011
 </t>
     </r>
   </si>
@@ -1141,33 +1028,6 @@
   <si>
     <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
   </si>
-  <si>
-    <t xml:space="preserve">ប៊ីប៉ូស្ទ័របង្អួចទីផ្សារថ្មី ក្លាហាន(Window-Klahan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ប៊ីប៉ូស្ទ័របង្អួចទីផ្សារថ្មី ប្រយុទ្ឋ(Window-Broyuth)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ទូរCBCនៅទីតាំង ខាងមុខគេ (KO Cooler First Position)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ទូរCBCបើក ប្រើប្រាស់ (KO Cooler Switch On)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ភាពសុទ្ធក្នុង ទូរCBC (KO Cooler Purity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ចំណែកមិនសុទ្ធ ក្នុងទូរCBC (Impure KO-Cooler)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ទូរCBC (KO Cooler)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ចំណែកផលិតផល ត្រជាក់(Cold SOVI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ចំណែកផលិតផល តាំងមិនត្រជាក់ (Ambient SOVI)</t>
-  </si>
 </sst>
 </file>
 
@@ -1181,7 +1041,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1304,15 +1164,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DaunPenh"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1349,14 +1202,8 @@
         <bgColor rgb="FFEDEDED"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="35">
+  <borders count="32">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1527,13 +1374,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
@@ -1561,24 +1401,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1634,7 +1460,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="95">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1879,11 +1705,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="24" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="25" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="25" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1891,20 +1717,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="5" borderId="27" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="25" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="26" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="27" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="5" borderId="28" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="5" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1915,7 +1733,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="5" borderId="30" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="28" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1927,10 +1745,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="5" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1939,7 +1753,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="5" borderId="32" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="5" borderId="29" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1951,7 +1765,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="33" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="17" fillId="3" borderId="30" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1963,7 +1777,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="34" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="31" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1971,15 +1785,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="5" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="5" borderId="30" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="5" borderId="28" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1995,10 +1805,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2011,15 +1817,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="5" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="5" borderId="32" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="5" borderId="29" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2119,31 +1921,31 @@
   </sheetPr>
   <dimension ref="1:39"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="1" sqref="C6:C12 D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="57.9514170040486"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="44.4534412955466"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="85.587044534413"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="86.336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.0607287449393"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="67.8056680161943"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="68.3400809716599"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.31983805668016"/>
@@ -34865,18 +34667,18 @@
   </sheetPr>
   <dimension ref="1:20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="C6:C12 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="22" width="3.74898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="22" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="22" width="3.74898785425101"/>
@@ -34886,7 +34688,7 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="22" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="22" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="22" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="22" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="22" width="4.2834008097166"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="22" width="4.92712550607287"/>
@@ -39094,7 +38896,7 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
         <v>29</v>
       </c>
@@ -39153,7 +38955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
         <v>31</v>
       </c>
@@ -39212,7 +39014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="37" t="s">
         <v>33</v>
       </c>
@@ -39944,14 +39746,14 @@
   </sheetPr>
   <dimension ref="B1:R8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C6:C12 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.24696356275304"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
@@ -39962,7 +39764,7 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="1" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.31983805668016"/>
@@ -40103,162 +39905,162 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="61" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="62" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="61" t="n">
         <v>1.25</v>
       </c>
-      <c r="D6" s="63" t="n">
+      <c r="D6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="64" t="n">
+      <c r="E6" s="63" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="62" t="n">
+      <c r="F6" s="61" t="n">
         <v>0.75</v>
       </c>
-      <c r="G6" s="65" t="n">
+      <c r="G6" s="64" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="65" t="n">
+      <c r="H6" s="64" t="n">
         <v>0.75</v>
       </c>
-      <c r="I6" s="65" t="n">
+      <c r="I6" s="64" t="n">
         <v>0.75</v>
       </c>
-      <c r="J6" s="65" t="n">
+      <c r="J6" s="64" t="n">
         <v>0.75</v>
       </c>
-      <c r="K6" s="65" t="n">
+      <c r="K6" s="64" t="n">
         <v>0.75</v>
       </c>
-      <c r="L6" s="63" t="n">
+      <c r="L6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="63" t="n">
+      <c r="M6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="63" t="n">
+      <c r="N6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="63" t="n">
+      <c r="O6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="P6" s="63" t="n">
+      <c r="P6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="63" t="n">
+      <c r="Q6" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="R6" s="66" t="n">
+      <c r="R6" s="65" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="68" t="n">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="66" t="n">
         <v>1.25</v>
       </c>
-      <c r="D7" s="69" t="n">
+      <c r="D7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="70" t="n">
+      <c r="E7" s="68" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="68" t="n">
+      <c r="F7" s="66" t="n">
         <v>0.75</v>
       </c>
-      <c r="G7" s="71" t="n">
+      <c r="G7" s="69" t="n">
         <v>0.75</v>
       </c>
-      <c r="H7" s="71" t="n">
+      <c r="H7" s="69" t="n">
         <v>0.75</v>
       </c>
-      <c r="I7" s="71" t="n">
+      <c r="I7" s="69" t="n">
         <v>0.75</v>
       </c>
-      <c r="J7" s="71" t="n">
+      <c r="J7" s="69" t="n">
         <v>0.75</v>
       </c>
-      <c r="K7" s="71" t="n">
+      <c r="K7" s="69" t="n">
         <v>0.75</v>
       </c>
-      <c r="L7" s="69" t="n">
+      <c r="L7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="69" t="n">
+      <c r="M7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="69" t="n">
+      <c r="N7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="69" t="n">
+      <c r="O7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="69" t="n">
+      <c r="P7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="69" t="n">
+      <c r="Q7" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="R7" s="72" t="n">
+      <c r="R7" s="70" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="74" t="n">
+      <c r="B8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="71" t="n">
         <v>2.5</v>
       </c>
-      <c r="D8" s="75" t="n">
+      <c r="D8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="76" t="n">
+      <c r="E8" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="74" t="n">
+      <c r="F8" s="71" t="n">
         <v>1.5</v>
       </c>
-      <c r="G8" s="77" t="n">
+      <c r="G8" s="74" t="n">
         <v>1.5</v>
       </c>
-      <c r="H8" s="77" t="n">
+      <c r="H8" s="74" t="n">
         <v>1.5</v>
       </c>
-      <c r="I8" s="77" t="n">
+      <c r="I8" s="74" t="n">
         <v>1.5</v>
       </c>
-      <c r="J8" s="77" t="n">
+      <c r="J8" s="74" t="n">
         <v>1.5</v>
       </c>
-      <c r="K8" s="77" t="n">
+      <c r="K8" s="74" t="n">
         <v>1.5</v>
       </c>
-      <c r="L8" s="75" t="n">
+      <c r="L8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="75" t="n">
+      <c r="M8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="N8" s="75" t="n">
+      <c r="N8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="75" t="n">
+      <c r="O8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="75" t="n">
+      <c r="P8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="75" t="n">
+      <c r="Q8" s="72" t="n">
         <v>0</v>
       </c>
-      <c r="R8" s="78" t="n">
+      <c r="R8" s="75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -40286,15 +40088,15 @@
   </sheetPr>
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6761133603239"/>
@@ -40306,7 +40108,7 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="9.31983805668016"/>
@@ -40376,7 +40178,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="53"/>
-      <c r="C4" s="79"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="55" t="s">
         <v>128</v>
       </c>
@@ -40399,13 +40201,13 @@
       <c r="S4" s="55"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="79" t="s">
         <v>132</v>
       </c>
       <c r="E5" s="58" t="s">
@@ -40454,395 +40256,395 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="83" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="84" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" s="85" t="n">
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="85" t="n">
+      <c r="E6" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="86" t="n">
+      <c r="F6" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="87" t="n">
+      <c r="G6" s="83" t="n">
         <v>0.5</v>
       </c>
-      <c r="H6" s="85" t="n">
+      <c r="H6" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="85" t="n">
+      <c r="I6" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="J6" s="85" t="n">
+      <c r="J6" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="K6" s="85" t="n">
+      <c r="K6" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="L6" s="85" t="n">
+      <c r="L6" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="M6" s="88" t="n">
+      <c r="M6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="N6" s="88" t="n">
+      <c r="N6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="O6" s="88" t="n">
+      <c r="O6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="P6" s="88" t="n">
+      <c r="P6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="88" t="n">
+      <c r="Q6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="R6" s="88" t="n">
+      <c r="R6" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="S6" s="89" t="n">
+      <c r="S6" s="85" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="83" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="84" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="85" t="n">
+      <c r="C7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="85" t="n">
+      <c r="E7" s="81" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="86" t="n">
+      <c r="F7" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="87" t="n">
+      <c r="G7" s="83" t="n">
         <v>0.5</v>
       </c>
-      <c r="H7" s="85" t="n">
+      <c r="H7" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="I7" s="85" t="n">
+      <c r="I7" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="J7" s="85" t="n">
+      <c r="J7" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="K7" s="85" t="n">
+      <c r="K7" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="L7" s="85" t="n">
+      <c r="L7" s="81" t="n">
         <v>0.5</v>
       </c>
-      <c r="M7" s="88" t="n">
+      <c r="M7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="N7" s="88" t="n">
+      <c r="N7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="O7" s="88" t="n">
+      <c r="O7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="P7" s="88" t="n">
+      <c r="P7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="88" t="n">
+      <c r="Q7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="R7" s="88" t="n">
+      <c r="R7" s="84" t="n">
         <v>0.5</v>
       </c>
-      <c r="S7" s="89" t="n">
+      <c r="S7" s="85" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="83" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="84" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="85" t="n">
+      <c r="C8" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="81" t="n">
         <v>2.5</v>
       </c>
-      <c r="E8" s="85" t="n">
+      <c r="E8" s="81" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="86" t="n">
+      <c r="F8" s="82" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="87" t="n">
+      <c r="G8" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="85" t="n">
+      <c r="H8" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="85" t="n">
+      <c r="I8" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="85" t="n">
+      <c r="J8" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="85" t="n">
+      <c r="K8" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="85" t="n">
+      <c r="L8" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="M8" s="88" t="n">
+      <c r="M8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="N8" s="88" t="n">
+      <c r="N8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="O8" s="88" t="n">
+      <c r="O8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="P8" s="88" t="n">
+      <c r="P8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="88" t="n">
+      <c r="Q8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="R8" s="88" t="n">
+      <c r="R8" s="84" t="n">
         <v>1.5</v>
       </c>
-      <c r="S8" s="89" t="n">
+      <c r="S8" s="85" t="n">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="83" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="85" t="n">
+      <c r="C9" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="85" t="n">
+      <c r="E9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="86" t="n">
+      <c r="F9" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="87" t="n">
+      <c r="G9" s="83" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="85" t="n">
+      <c r="H9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="85" t="n">
+      <c r="I9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="85" t="n">
+      <c r="J9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="85" t="n">
+      <c r="K9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="85" t="n">
+      <c r="L9" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="88" t="n">
+      <c r="M9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="88" t="n">
+      <c r="N9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="88" t="n">
+      <c r="O9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="88" t="n">
+      <c r="P9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="88" t="n">
+      <c r="Q9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="R9" s="88" t="n">
+      <c r="R9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="S9" s="89" t="n">
+      <c r="S9" s="85" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="83" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="90" t="s">
-        <v>189</v>
-      </c>
-      <c r="D10" s="85" t="n">
+      <c r="C10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="85" t="n">
+      <c r="E10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="86" t="n">
+      <c r="F10" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="87" t="n">
+      <c r="G10" s="83" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="85" t="n">
+      <c r="H10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="85" t="n">
+      <c r="I10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="85" t="n">
+      <c r="J10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="85" t="n">
+      <c r="K10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="85" t="n">
+      <c r="L10" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="88" t="n">
+      <c r="M10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="N10" s="88" t="n">
+      <c r="N10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="88" t="n">
+      <c r="O10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="88" t="n">
+      <c r="P10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="88" t="n">
+      <c r="Q10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="R10" s="88" t="n">
+      <c r="R10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="S10" s="89" t="n">
+      <c r="S10" s="85" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="83" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="85" t="n">
+      <c r="C11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="81" t="n">
         <v>2.5</v>
       </c>
-      <c r="E11" s="85" t="n">
+      <c r="E11" s="81" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="86" t="n">
+      <c r="F11" s="82" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="91" t="n">
+      <c r="G11" s="86" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="92" t="n">
+      <c r="H11" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="92" t="n">
+      <c r="I11" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="J11" s="92" t="n">
+      <c r="J11" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="92" t="n">
+      <c r="K11" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="L11" s="92" t="n">
+      <c r="L11" s="87" t="n">
         <v>2</v>
       </c>
-      <c r="M11" s="92" t="n">
+      <c r="M11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="92" t="n">
+      <c r="N11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="92" t="n">
+      <c r="O11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="P11" s="92" t="n">
+      <c r="P11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="92" t="n">
+      <c r="Q11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="R11" s="92" t="n">
+      <c r="R11" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="S11" s="93" t="n">
+      <c r="S11" s="88" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="83" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="94" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="95" t="n">
+      <c r="C12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="89" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="95" t="n">
+      <c r="E12" s="89" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="96" t="n">
+      <c r="F12" s="90" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="97" t="n">
+      <c r="G12" s="91" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="98" t="n">
+      <c r="H12" s="92" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="98" t="n">
+      <c r="I12" s="92" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="98" t="n">
+      <c r="J12" s="92" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="98" t="n">
+      <c r="K12" s="92" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="98" t="n">
+      <c r="L12" s="92" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="99" t="s">
+      <c r="M12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="N12" s="99" t="s">
+      <c r="N12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="O12" s="99" t="s">
+      <c r="O12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="P12" s="99" t="s">
+      <c r="P12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="Q12" s="99" t="s">
+      <c r="Q12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="R12" s="99" t="s">
+      <c r="R12" s="93" t="s">
         <v>166</v>
       </c>
-      <c r="S12" s="100" t="s">
+      <c r="S12" s="94" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-6544 - CCKH - Template update - SKU update effective 6th Oct 2018
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -884,65 +884,32 @@
     <t xml:space="preserve">Club</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coca Cola Coffee 330ml,Coke 240ml,Coca-cola 250ml Can,Coke Vanilla 330ml
+    <t xml:space="preserve">Coca Cola 330ml,Coca Cola 390ml,Coca Cola Light 330ml,Coca Cola Zero 330ml Can,Coca Cola 500ml,Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coca Cola Coffee 330ml,Coca Cola 350ml
 </t>
-    </r>
   </si>
   <si>
-    <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,88471005623958851959905876,8847100562999,8847100565495</t>
+    <t xml:space="preserve">8847100562746,8847100567574,8847100566898,8847100565389,8847100562715,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,847100562234_4,8847100562234_5,8847100562395,8847100561015</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprite 330ml Can,Sprite Zero 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET,Sprite 330ml Sleek Can,Sprite 240ml Slim Can,Sprite 250ml Can</t>
+    <t xml:space="preserve">Sprite 330ml Can,Sprite Zero 330ml Can,Sprite 390ml PET,Sprite 450ml PET,Sprite 500ml PET,Sprite 330ml Sleek Can,Sprite 350ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100561459,8847100562364,8847100563736,8851959905944,8847100562104,8847100568793,8851959905906,8847100568847</t>
+    <t xml:space="preserve">8847100561459,8851959905944,8847100563736,8847100562104,8847100562364,8847100568793,8847100561022</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Orange 330ml,Fanta Orange 390ml,Fanta Orange 500ml,Fanta Orange 240ml Slim Can,Fanta Orange 250ml Can
+    <t xml:space="preserve">Fanta Orange 330ml,Fanta Orange 390ml,Fanta Orange 500ml,Fanta Orange 350ml
 </t>
-    </r>
   </si>
   <si>
-    <t xml:space="preserve">8847100560094,8847100561244,8847100564603,
-8851959905883,8847100564799</t>
+    <t xml:space="preserve">8847100560094,8847100561244,8847100564603,8847100561039_0</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 390ml,Fanta Fruit Punch 330ml Sleek Can,Fanta Fruit Punch 240ml Slim Can,Fanta Fruit Punch 250ml Can
+    <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 390ml,Fanta Fruit Punch 350ml
 </t>
-    </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8847100564061,8847100564184,8847100564061,8851959133187,8847100569011
+    <t xml:space="preserve">8847100564061,8847100564184,8847100561046_0
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Fanta Redberry 330ml,Fanta Blueberry 330ml,Fanta Blueberry 390ml,Fanta Grape  330ml,Fanta Redberry 330ml,Fanta Blueberry 330ml, Fanta +C 390ml,Fanta +C 330ml
@@ -953,16 +920,17 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Samurai Strawberry 330ml,Samurai Fruity 330ml,Samurai Strawberry 480ml,Samurai Fruity 480ml,Mutant Green 330ml Can,Mutant Yellow 330ml Can,Mutant Yellow 400ml PET,Mutant Green 400ml PET,Mutant Red 330ml Can  Mutant Red 400ml PET,Samurai Strawberry 390 PET,Samurai Fruity 390 PET,Samurai Strawberry 330 Sleek Can,Samurai Fruity 330 Sleek Can</t>
+    <t xml:space="preserve">Samurai Strawberry 330ml,Samurai Fruity 330ml,Samurai Strawberry 480ml,Samurai Fruity 480ml,Mutant Green 330ml Can,Mutant Black 330ml Can,Mutant Green 400ml PET,Mutant Yellow 400ml PET,Mutant Red 330ml Can,Mutant Red 400ml PET,Thunder Strawberry 330ml,Thunder Strawberry 480ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100566591,8847100566607,8847100566874,8847100566676,8847100566650,8847100568601,8847100568595,8847100568618,8847100565943,8847100565952,8847100566478,8847100567079,8847100566867,8847100567864</t>
+    <t xml:space="preserve">8847100566591,8847100566607,8847100566874,8847100566676,8847100566650,8847100568601,8847100568595,8847100568618,8847100565943,8847100565952,8847100561091,8847100561152</t>
   </si>
   <si>
-    <t xml:space="preserve">Dasani 350ml,Dasani 500ml,Dasani 1.5L PET,Dasani 550ml,Dasani Mineral 500ml</t>
+    <t xml:space="preserve">Dasani 350ml,Dasani 500ml,Dasani 1.5L PET,Dasani 550ml,Dasani Mineral 500ml,
+Dasani 550ml</t>
   </si>
   <si>
-    <t xml:space="preserve">8847100560025,8847100568526,8847100562111,8851959905999,8847100567784</t>
+    <t xml:space="preserve">8847100560025,8847100568526,8847100562111,8851959905999,8847100567784,8847100568526_0</t>
   </si>
   <si>
     <t xml:space="preserve">Aquarius 330ml Can,Aquarius 330ml Sleek Can,Aquarius 390ml PET,Aquarius Veggies 330ml Can</t>
@@ -1041,7 +1009,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1132,13 +1100,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1597,11 +1558,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1621,15 +1582,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1637,7 +1598,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1649,11 +1610,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1673,15 +1634,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1765,7 +1726,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="30" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="30" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1924,28 +1885,28 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D19" activeCellId="1" sqref="C6:C12 D19"/>
+      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.4858299595142"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="86.336032388664"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="87.0890688259109"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="33.8502024291498"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="68.3400809716599"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="68.8785425101215"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.31983805668016"/>
@@ -34667,18 +34628,18 @@
   </sheetPr>
   <dimension ref="1:20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="C6:C12 D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="22" width="3.74898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="22" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="22" width="3.74898785425101"/>
@@ -34688,7 +34649,7 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="22" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="22" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="22" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="22" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="22" width="4.2834008097166"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="22" width="4.92712550607287"/>
@@ -38834,7 +38795,7 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
     </row>
-    <row r="6" s="36" customFormat="true" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="36" customFormat="true" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="31" t="s">
         <v>22</v>
@@ -38955,7 +38916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
         <v>31</v>
       </c>
@@ -39014,7 +38975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="40.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="37" t="s">
         <v>33</v>
       </c>
@@ -39132,7 +39093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
         <v>37</v>
       </c>
@@ -39747,13 +39708,13 @@
   <dimension ref="B1:R8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C6:C12 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.24696356275304"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6761133603239"/>
@@ -39764,7 +39725,7 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="1" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.31983805668016"/>
@@ -40088,15 +40049,15 @@
   </sheetPr>
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6:C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6761133603239"/>
@@ -40108,7 +40069,7 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="9.31983805668016"/>

</xml_diff>

<commit_message>
PROS-7920 - Template change - store_type changed from 'KH-Canteen-Edu/Fact_Gold' to 'KH-Canteen-Edu/Fact._Gold'
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="272">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -889,310 +889,313 @@
     <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Gold</t>
   </si>
   <si>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact._Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Stalls_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Entertainment_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-GH./Mini-Hotel_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Café Shop_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Internet/E-Game_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-KTV/Night Club_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Mobile Premix_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Massage/Spa_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Fitness Center_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Sport Club_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Drinking Stalls_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-At Work/Offices_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Cinema_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-CVS_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Court_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Hotel(4Stars Up)_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-QSR_Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Restaurants_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Stalls_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Entertainment_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-GH./Mini-Hotel_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Café Shop_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Internet/E-Game_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-KTV/Night Club_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Mobile Premix_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Massage/Spa_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Fitness Center_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Sport Club_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Drinking Stalls_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-At Work/Offices_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Cinema_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-CVS_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Court_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Hotel(4Stars Up)_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-QSR_Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Restaurants_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Stalls_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Entertainment_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-GH./Mini-Hotel_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Café Shop_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Internet/E-Game_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-KTV/Night Club_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Mobile Premix_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Massage/Spa_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Fitness Center_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Sport Club_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Drinking Stalls_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-At Work/Offices_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Cinema_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-CVS_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Food Court_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-Hotel(4Stars Up)_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH-QSR_Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coke 330ml, Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coke 330ml_Cx24 PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100562234,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,8847100562234_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100562395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppe Soda 330ml Can, Schweppe Soda 330ml Sleek Can, Schweppe Soda 330ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100563026,8847100563897,8847100563897_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca Cola 600ml,Coke 600ml_Cx24 PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100563637,8847100563537_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange 330ml,Fanta orange 330ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100560094,8847100567376_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 330ml Sleek Can,Fanta Fruit Punch 330ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100564061_d,8847100564061,8847100564061_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite 330ml Can,Sprite 330ml Sleek Can,Sprite 330ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561459,8847100568793,8847100568793_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Tea Green Tea Honey 350ml,Fuze Tea Peach Black Tea 350ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561411,8847100561404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca Cola 1.5L,Coke 1.5L_CX6 PACK,Coke 2.25L_C X6 PACK,Coca Cola 2.25L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8935049500117,8847100561084_C,8847100560568_C,8847100560568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange 1.5L,Fanta Orange 2.25L,Fanta orange 1.5L_C X6 PACK,Fanta Orange 2.25L_C X6PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100560896,8847100560926,8847100560896_C,8847100560926_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Fruit Punch 1.5L,Fanta Fruit Punch 2.25L,Fanta Fruit Punch 1.5L_C X6PACK,Fanta Fruit Punch 2.25L_C X6 PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100564979,8847100562258,8847100564979_C,8847100562258_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Blueberry 1.5L,Fanta Grape 1.5L PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100568830,8847100563149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite 1.5L,Sprite 2.25L,Sprite 1.5L_C X6 PACK,Sprite 2.25L_C X6 PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100560902,8847100560919,8847100560902_C,8847100560919_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minute Maid Grape Can 330ml,Minute Maid Refresh Apple Can,Minute Maid Grape 330ml_C X24PACK,Minute Maid Orange Mango 330ml Can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100569837,8847100562951,8847100569837_C,8847100562388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutant Green 330ml Can,Mutant Green 400ml PET,Mutant Yellow 330ml Can,Mutant Yellow 400ml P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100566650,8847100568618,8847100568601,8847100568595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutant Red 330ml Can,Mutant Red 400ml PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100565943,8847100565952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Strawberry 330ml,Thunder Strawberry 480ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561091,8847100561152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquarius 330ml Can, Aquarius 330ml Sleek Can,Aquarius 390ml PET, Aquarius Veggies 330ml Can,Aquarius 330ml_C X24PACK, Aquarius 390ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100561237,8847100568960,8847100563170,8847100562272,8847100568960_C,8847100563170_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dasani 500ml,Dasani 500ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100568526,8847100568526_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dasani Mineral 500ml,Dasani Mineral 500ml_C X24PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100567784,8847100567784_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dasani 1.5L PET,Dasani 1.5L_C X6PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8847100562111,8847100562111_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
+  </si>
+  <si>
     <t xml:space="preserve">KH-Canteen-Edu/Fact_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Stalls_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Entertainment_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-GH./Mini-Hotel_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Café Shop_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Internet/E-Game_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-KTV/Night Club_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Mobile Premix_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Massage/Spa_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Fitness Center_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Sport Club_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Drinking Stalls_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-At Work/Offices_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Cinema_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-CVS_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Court_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Hotel(4Stars Up)_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-QSR_Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Restaurants_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Stalls_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Entertainment_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-GH./Mini-Hotel_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Café Shop_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Internet/E-Game_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-KTV/Night Club_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Mobile Premix_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Massage/Spa_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Fitness Center_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Sport Club_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Drinking Stalls_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-At Work/Offices_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Cinema_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-CVS_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Court_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Hotel(4Stars Up)_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-QSR_Silver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Restaurants_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Stalls_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Entertainment_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-GH./Mini-Hotel_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Café Shop_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Internet/E-Game_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-KTV/Night Club_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Mobile Premix_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Massage/Spa_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Fitness Center_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Sport Club_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Drinking Stalls_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-At Work/Offices_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Cinema_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-CVS_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Food Court_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Hotel(4Stars Up)_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-QSR_Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coke 330ml, Coke ARG 330ml,Coke BRA 330ml,Coke FRA 330ml,Coke GER 330ml,Coke POR 330ml,Coke ESP 330ml,Coke 330ml_Cx24 PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100562234,8847100562234_0,8847100562234_1,8847100562234_2,8847100562234_3,8847100562234_4,8847100562234_5,8847100562234_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100562395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppe Soda 330ml Can, Schweppe Soda 330ml Sleek Can, Schweppe Soda 330ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100563026,8847100563897,8847100563897_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100561015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca Cola 600ml,Coke 600ml_Cx24 PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100563637,8847100563537_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange 330ml,Fanta orange 330ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100560094,8847100567376_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Fruit Punch 330ml,Fanta Fruit Punch 330ml Sleek Can,Fanta Fruit Punch 330ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100564061_d,8847100564061,8847100564061_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite 330ml Can,Sprite 330ml Sleek Can,Sprite 330ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100561459,8847100568793,8847100568793_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Tea Green Tea Honey 350ml,Fuze Tea Peach Black Tea 350ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100561411,8847100561404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca Cola 1.5L,Coke 1.5L_CX6 PACK,Coke 2.25L_C X6 PACK,Coca Cola 2.25L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8935049500117,8847100561084_C,8847100560568_C,8847100560568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange 1.5L,Fanta Orange 2.25L,Fanta orange 1.5L_C X6 PACK,Fanta Orange 2.25L_C X6PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100560896,8847100560926,8847100560896_C,8847100560926_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Fruit Punch 1.5L,Fanta Fruit Punch 2.25L,Fanta Fruit Punch 1.5L_C X6PACK,Fanta Fruit Punch 2.25L_C X6 PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100564979,8847100562258,8847100564979_C,8847100562258_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Blueberry 1.5L,Fanta Grape 1.5L PET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100568830,8847100563149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite 1.5L,Sprite 2.25L,Sprite 1.5L_C X6 PACK,Sprite 2.25L_C X6 PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100560902,8847100560919,8847100560902_C,8847100560919_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minute Maid Grape Can 330ml,Minute Maid Refresh Apple Can,Minute Maid Grape 330ml_C X24PACK,Minute Maid Orange Mango 330ml Can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100569837,8847100562951,8847100569837_C,8847100562388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutant Green 330ml Can,Mutant Green 400ml PET,Mutant Yellow 330ml Can,Mutant Yellow 400ml P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100566650,8847100568618,8847100568601,8847100568595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutant Red 330ml Can,Mutant Red 400ml PET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100565943,8847100565952</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thunder Strawberry 330ml,Thunder Strawberry 480ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100561091,8847100561152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aquarius 330ml Can, Aquarius 330ml Sleek Can,Aquarius 390ml PET, Aquarius Veggies 330ml Can,Aquarius 330ml_C X24PACK, Aquarius 390ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100561237,8847100568960,8847100563170,8847100562272,8847100568960_C,8847100563170_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dasani 500ml,Dasani 500ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100568526,8847100568526_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dasani Mineral 500ml,Dasani Mineral 500ml_C X24PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100567784,8847100567784_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dasani 1.5L PET,Dasani 1.5L_C X6PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8847100562111,8847100562111_C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
   </si>
 </sst>
 </file>
@@ -1871,23 +1874,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.5910931174089"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.1578947368421"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.1255060728745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.165991902834"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="68.7692307692308"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -3747,96 +3750,96 @@
   <dimension ref="1:27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="111.51012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="134.004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="112.582995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="135.182186234818"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="22" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="63" min="63" style="22" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="66" min="66" style="22" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1022" min="87" style="22" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
   </cols>
@@ -12864,88 +12867,88 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="43" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="64" min="64" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="85" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -13372,7 +13375,7 @@
         <v>168</v>
       </c>
       <c r="AA5" s="49" t="s">
-        <v>169</v>
+        <v>271</v>
       </c>
       <c r="AB5" s="49" t="s">
         <v>170</v>
@@ -14331,89 +14334,89 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="43" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="86" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -18608,7 +18611,7 @@
         <v>168</v>
       </c>
       <c r="AB5" s="57" t="s">
-        <v>169</v>
+        <v>271</v>
       </c>
       <c r="AC5" s="57" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
PROS-7427 CCANZ Inclusion and Exclusion
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="271">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -1193,9 +1193,6 @@
   </si>
   <si>
     <t xml:space="preserve">Weight Per Store Types (N/A - do not run KPI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Gold</t>
   </si>
 </sst>
 </file>
@@ -1868,29 +1865,29 @@
   </sheetPr>
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4534412955466"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.1578947368421"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.1255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.9068825910931"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.7692307692308"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="69.412955465587"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -3749,97 +3746,97 @@
   </sheetPr>
   <dimension ref="1:27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC5" activeCellId="0" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="112.582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="135.182186234818"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="113.546558704453"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="136.46963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="22" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="63" min="63" style="22" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="66" min="66" style="22" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1022" min="87" style="22" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
   </cols>
@@ -12860,95 +12857,95 @@
   </sheetPr>
   <dimension ref="B1:CF8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="43" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="64" min="64" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="85" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -13375,7 +13372,7 @@
         <v>168</v>
       </c>
       <c r="AA5" s="49" t="s">
-        <v>271</v>
+        <v>169</v>
       </c>
       <c r="AB5" s="49" t="s">
         <v>170</v>
@@ -14326,97 +14323,97 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB5" activeCellId="0" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="43" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="86" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -18611,7 +18608,7 @@
         <v>168</v>
       </c>
       <c r="AB5" s="57" t="s">
-        <v>271</v>
+        <v>169</v>
       </c>
       <c r="AC5" s="57" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
PROS-7920 CCKH StoreType update
</commit_message>
<xml_diff>
--- a/Projects/CCKH/Data/Template.xlsx
+++ b/Projects/CCKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -949,7 +949,7 @@
     <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Silver</t>
   </si>
   <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Silver</t>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact._Silver</t>
   </si>
   <si>
     <t xml:space="preserve">KH-Food Stalls_Silver</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">KH-BBQ/Soup/Beer Gdn_Bronze</t>
   </si>
   <si>
-    <t xml:space="preserve">KH-Canteen-Edu/Fact_Bronze</t>
+    <t xml:space="preserve">KH-Canteen-Edu/Fact._Bronze</t>
   </si>
   <si>
     <t xml:space="preserve">KH-Food Stalls_Bronze</t>
@@ -1865,29 +1865,29 @@
   </sheetPr>
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.9068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.7692307692308"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="97.4777327935223"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -3746,97 +3746,97 @@
   </sheetPr>
   <dimension ref="1:27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC5" activeCellId="0" sqref="AC5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW6" activeCellId="0" sqref="AW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="113.546558704453"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="136.46963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="116.651821862348"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="140.113360323887"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="22" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="22" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="22" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="22" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="22" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="22" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="22" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="22" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="22" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="22" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="22" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="22" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="22" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="22" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="22" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="22" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="22" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="22" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="22" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="22" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="22" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="22" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="22" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="22" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="22" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="22" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="22" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="22" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="22" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="22" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="22" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="22" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="22" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="22" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="22" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="22" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="22" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="22" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="63" min="63" style="22" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="22" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="22" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="66" min="66" style="22" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="22" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="22" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="22" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="22" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="22" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="22" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="22" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="22" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="22" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="22" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="22" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="22" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="22" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="22" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="22" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="22" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="22" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="22" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="22" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1022" min="87" style="22" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
   </cols>
@@ -12857,95 +12857,95 @@
   </sheetPr>
   <dimension ref="B1:CF8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AU6" activeCellId="0" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="44" min="44" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="43" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="64" min="64" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="85" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -14323,97 +14323,97 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB5" activeCellId="0" sqref="AB5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV5" activeCellId="0" sqref="AV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="43" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="43" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="43" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="43" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="43" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="43" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="43" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="43" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="43" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="43" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="43" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="43" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="43" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="43" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="43" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="43" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="43" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="43" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="43" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="43" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="43" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="43" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="43" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="43" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="43" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="43" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="43" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="43" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="43" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="43" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="43" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="43" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="43" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="43" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="43" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="43" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="43" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="43" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="43" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="43" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="72" min="72" style="43" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="43" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="74" min="74" style="43" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="75" min="75" style="43" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="43" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="43" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="43" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="79" min="79" style="43" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="43" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="43" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="43" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="43" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="43" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="43" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="86" style="43" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>